<commit_message>
Update 30 aug 2018
</commit_message>
<xml_diff>
--- a/conf/SensorsInLab.xlsx
+++ b/conf/SensorsInLab.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TME230\Documents\MATLAB\abraDAQ\conf\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="16275" windowHeight="11310"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="75">
   <si>
     <t>Calibration settings for available sensors</t>
   </si>
@@ -317,15 +322,18 @@
   <si>
     <t>None</t>
   </si>
+  <si>
+    <t>352A24</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,6 +543,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -581,7 +597,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -613,9 +629,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -647,6 +664,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -822,14 +840,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N100"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="I90" sqref="I90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.28515625" customWidth="1"/>
@@ -844,7 +862,7 @@
     <col min="14" max="14" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75">
+    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,7 +880,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75">
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -878,7 +896,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="17.25">
+    <row r="3" spans="1:14" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
@@ -914,7 +932,7 @@
       <c r="M3" s="6"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="9"/>
       <c r="C4" s="10" t="s">
@@ -948,7 +966,7 @@
       <c r="M4" s="6"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
@@ -985,7 +1003,7 @@
       <c r="M5" s="6"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10" t="s">
@@ -1022,7 +1040,7 @@
       <c r="M6" s="6"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
@@ -1059,7 +1077,7 @@
       <c r="M7" s="6"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10" t="s">
@@ -1096,7 +1114,7 @@
       <c r="M8" s="6"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
@@ -1133,7 +1151,7 @@
       <c r="M9" s="6"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10" t="s">
@@ -1167,7 +1185,7 @@
       <c r="M10" s="6"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
@@ -1201,7 +1219,7 @@
       <c r="M11" s="6"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10" t="s">
@@ -1235,7 +1253,7 @@
       <c r="M12" s="6"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
@@ -1261,7 +1279,7 @@
         <v>1.0550458715596329E-2</v>
       </c>
       <c r="J13" s="11">
-        <f>1/I13</f>
+        <f t="shared" ref="J13:J44" si="0">1/I13</f>
         <v>94.782608695652186</v>
       </c>
       <c r="K13" s="8">
@@ -1271,7 +1289,7 @@
       <c r="M13" s="6"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10" t="s">
@@ -1297,7 +1315,7 @@
         <v>1.0356778797145768E-2</v>
       </c>
       <c r="J14" s="11">
-        <f>1/I14</f>
+        <f t="shared" si="0"/>
         <v>96.555118110236236</v>
       </c>
       <c r="K14" s="8">
@@ -1307,7 +1325,7 @@
       <c r="M14" s="6"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10" t="s">
@@ -1333,7 +1351,7 @@
         <v>1.0183486238532109E-2</v>
       </c>
       <c r="J15" s="11">
-        <f>1/I15</f>
+        <f t="shared" si="0"/>
         <v>98.198198198198213</v>
       </c>
       <c r="K15" s="8">
@@ -1343,7 +1361,7 @@
       <c r="M15" s="6"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10" t="s">
@@ -1369,7 +1387,7 @@
         <v>1.0122324159021406E-2</v>
       </c>
       <c r="J16" s="11">
-        <f>1/I16</f>
+        <f t="shared" si="0"/>
         <v>98.791540785498498</v>
       </c>
       <c r="K16" s="8">
@@ -1379,7 +1397,7 @@
       <c r="M16" s="6"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10" t="s">
@@ -1405,7 +1423,7 @@
         <v>9.6636085626911311E-4</v>
       </c>
       <c r="J17" s="11">
-        <f>1/I17</f>
+        <f t="shared" si="0"/>
         <v>1034.8101265822786</v>
       </c>
       <c r="K17" s="8">
@@ -1415,7 +1433,7 @@
       <c r="M17" s="6"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10" t="s">
@@ -1440,7 +1458,7 @@
         <v>1.0290000000000001E-2</v>
       </c>
       <c r="J18" s="11">
-        <f>1/I18</f>
+        <f t="shared" si="0"/>
         <v>97.181729834791057</v>
       </c>
       <c r="K18" s="8">
@@ -1450,7 +1468,7 @@
       <c r="M18" s="6"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10" t="s">
@@ -1475,7 +1493,7 @@
         <v>1.1010000000000001E-2</v>
       </c>
       <c r="J19" s="11">
-        <f>1/I19</f>
+        <f t="shared" si="0"/>
         <v>90.826521344232503</v>
       </c>
       <c r="K19" s="8">
@@ -1485,7 +1503,7 @@
       <c r="M19" s="6"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10" t="s">
@@ -1510,7 +1528,7 @@
         <v>1.017E-2</v>
       </c>
       <c r="J20" s="11">
-        <f>1/I20</f>
+        <f t="shared" si="0"/>
         <v>98.328416912487711</v>
       </c>
       <c r="K20" s="8">
@@ -1520,7 +1538,7 @@
       <c r="M20" s="6"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="9"/>
       <c r="C21" s="10" t="s">
@@ -1545,7 +1563,7 @@
         <v>1.0970000000000001E-2</v>
       </c>
       <c r="J21" s="11">
-        <f>1/I21</f>
+        <f t="shared" si="0"/>
         <v>91.157702825888776</v>
       </c>
       <c r="K21" s="8">
@@ -1555,7 +1573,7 @@
       <c r="M21" s="6"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
@@ -1581,7 +1599,7 @@
         <v>9.999999999999998E-4</v>
       </c>
       <c r="J22" s="11">
-        <f>1/I22</f>
+        <f t="shared" si="0"/>
         <v>1000.0000000000002</v>
       </c>
       <c r="K22" s="8">
@@ -1591,7 +1609,7 @@
       <c r="M22" s="6"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="9"/>
       <c r="C23" s="10" t="s">
@@ -1616,7 +1634,7 @@
         <v>1.008E-3</v>
       </c>
       <c r="J23" s="11">
-        <f>1/I23</f>
+        <f t="shared" si="0"/>
         <v>992.06349206349205</v>
       </c>
       <c r="K23" s="8">
@@ -1626,7 +1644,7 @@
       <c r="M23" s="6"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10" t="s">
@@ -1651,7 +1669,7 @@
         <v>9.6900000000000003E-4</v>
       </c>
       <c r="J24" s="11">
-        <f>1/I24</f>
+        <f t="shared" si="0"/>
         <v>1031.9917440660474</v>
       </c>
       <c r="K24" s="8">
@@ -1661,7 +1679,7 @@
       <c r="M24" s="6"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10" t="s">
@@ -1686,7 +1704,7 @@
         <v>9.6900000000000003E-4</v>
       </c>
       <c r="J25" s="11">
-        <f>1/I25</f>
+        <f t="shared" si="0"/>
         <v>1031.9917440660474</v>
       </c>
       <c r="K25" s="8">
@@ -1696,7 +1714,7 @@
       <c r="M25" s="6"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10" t="s">
@@ -1721,7 +1739,7 @@
         <v>1.026E-3</v>
       </c>
       <c r="J26" s="11">
-        <f>1/I26</f>
+        <f t="shared" si="0"/>
         <v>974.65886939571146</v>
       </c>
       <c r="K26" s="8">
@@ -1731,7 +1749,7 @@
       <c r="M26" s="6"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="9"/>
       <c r="C27" s="10" t="s">
@@ -1756,7 +1774,7 @@
         <v>1.0070000000000001E-3</v>
       </c>
       <c r="J27" s="11">
-        <f>1/I27</f>
+        <f t="shared" si="0"/>
         <v>993.04865938430976</v>
       </c>
       <c r="K27" s="8">
@@ -1766,7 +1784,7 @@
       <c r="M27" s="6"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10" t="s">
@@ -1791,7 +1809,7 @@
         <v>9.7900000000000005E-4</v>
       </c>
       <c r="J28" s="11">
-        <f>1/I28</f>
+        <f t="shared" si="0"/>
         <v>1021.4504596527067</v>
       </c>
       <c r="K28" s="8">
@@ -1801,7 +1819,7 @@
       <c r="M28" s="6"/>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="9"/>
       <c r="C29" s="10" t="s">
@@ -1826,7 +1844,7 @@
         <v>9.4799999999999995E-4</v>
       </c>
       <c r="J29" s="11">
-        <f>1/I29</f>
+        <f t="shared" si="0"/>
         <v>1054.8523206751056</v>
       </c>
       <c r="K29" s="8">
@@ -1836,7 +1854,7 @@
       <c r="M29" s="6"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10" t="s">
@@ -1861,7 +1879,7 @@
         <v>9.6000000000000002E-4</v>
       </c>
       <c r="J30" s="11">
-        <f>1/I30</f>
+        <f t="shared" si="0"/>
         <v>1041.6666666666667</v>
       </c>
       <c r="K30" s="8">
@@ -1871,7 +1889,7 @@
       <c r="M30" s="6"/>
       <c r="N30" s="2"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="9"/>
       <c r="C31" s="10" t="s">
@@ -1896,7 +1914,7 @@
         <v>9.859999999999999E-4</v>
       </c>
       <c r="J31" s="11">
-        <f>1/I31</f>
+        <f t="shared" si="0"/>
         <v>1014.1987829614606</v>
       </c>
       <c r="K31" s="8">
@@ -1906,7 +1924,7 @@
       <c r="M31" s="6"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="9"/>
       <c r="C32" s="10" t="s">
@@ -1931,7 +1949,7 @@
         <v>9.9799999999999997E-4</v>
       </c>
       <c r="J32" s="11">
-        <f>1/I32</f>
+        <f t="shared" si="0"/>
         <v>1002.0040080160321</v>
       </c>
       <c r="K32" s="8">
@@ -1941,7 +1959,7 @@
       <c r="M32" s="6"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="9"/>
       <c r="C33" s="10" t="s">
@@ -1966,7 +1984,7 @@
         <v>9.7599999999999998E-4</v>
       </c>
       <c r="J33" s="11">
-        <f>1/I33</f>
+        <f t="shared" si="0"/>
         <v>1024.5901639344263</v>
       </c>
       <c r="K33" s="8">
@@ -1976,7 +1994,7 @@
       <c r="M33" s="6"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="9"/>
       <c r="C34" s="10" t="s">
@@ -2001,7 +2019,7 @@
         <v>9.9500000000000001E-4</v>
       </c>
       <c r="J34" s="11">
-        <f>1/I34</f>
+        <f t="shared" si="0"/>
         <v>1005.0251256281407</v>
       </c>
       <c r="K34" s="8">
@@ -2011,7 +2029,7 @@
       <c r="M34" s="6"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="9"/>
       <c r="C35" s="10" t="s">
@@ -2036,7 +2054,7 @@
         <v>9.7999999999999997E-4</v>
       </c>
       <c r="J35" s="11">
-        <f>1/I35</f>
+        <f t="shared" si="0"/>
         <v>1020.4081632653061</v>
       </c>
       <c r="K35" s="8">
@@ -2046,7 +2064,7 @@
       <c r="M35" s="6"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="9"/>
       <c r="C36" s="10" t="s">
@@ -2071,7 +2089,7 @@
         <v>9.5399999999999999E-4</v>
       </c>
       <c r="J36" s="11">
-        <f>1/I36</f>
+        <f t="shared" si="0"/>
         <v>1048.2180293501049</v>
       </c>
       <c r="K36" s="8">
@@ -2081,7 +2099,7 @@
       <c r="M36" s="6"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="9"/>
       <c r="C37" s="10" t="s">
@@ -2106,7 +2124,7 @@
         <v>9.8499999999999998E-4</v>
       </c>
       <c r="J37" s="11">
-        <f>1/I37</f>
+        <f t="shared" si="0"/>
         <v>1015.2284263959391</v>
       </c>
       <c r="K37" s="8">
@@ -2116,7 +2134,7 @@
       <c r="M37" s="6"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="9"/>
       <c r="C38" s="10" t="s">
@@ -2141,7 +2159,7 @@
         <v>1.003E-3</v>
       </c>
       <c r="J38" s="11">
-        <f>1/I38</f>
+        <f t="shared" si="0"/>
         <v>997.00897308075776</v>
       </c>
       <c r="K38" s="8">
@@ -2151,7 +2169,7 @@
       <c r="M38" s="6"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="9"/>
       <c r="C39" s="10" t="s">
@@ -2176,7 +2194,7 @@
         <v>1.077E-3</v>
       </c>
       <c r="J39" s="11">
-        <f>1/I39</f>
+        <f t="shared" si="0"/>
         <v>928.50510677808722</v>
       </c>
       <c r="K39" s="8">
@@ -2186,7 +2204,7 @@
       <c r="M39" s="6"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="9"/>
       <c r="C40" s="10" t="s">
@@ -2211,7 +2229,7 @@
         <v>1.077E-3</v>
       </c>
       <c r="J40" s="11">
-        <f>1/I40</f>
+        <f t="shared" si="0"/>
         <v>928.50510677808722</v>
       </c>
       <c r="K40" s="8">
@@ -2221,7 +2239,7 @@
       <c r="M40" s="6"/>
       <c r="N40" s="2"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="9"/>
       <c r="C41" s="10" t="s">
@@ -2246,7 +2264,7 @@
         <v>1.039E-3</v>
       </c>
       <c r="J41" s="11">
-        <f>1/I41</f>
+        <f t="shared" si="0"/>
         <v>962.46390760346492</v>
       </c>
       <c r="K41" s="8">
@@ -2256,7 +2274,7 @@
       <c r="M41" s="6"/>
       <c r="N41" s="2"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="9"/>
       <c r="C42" s="10" t="s">
@@ -2281,7 +2299,7 @@
         <v>1.0629999999999999E-3</v>
       </c>
       <c r="J42" s="11">
-        <f>1/I42</f>
+        <f t="shared" si="0"/>
         <v>940.73377234242719</v>
       </c>
       <c r="K42" s="8">
@@ -2291,7 +2309,7 @@
       <c r="M42" s="6"/>
       <c r="N42" s="2"/>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="9"/>
       <c r="C43" s="10" t="s">
@@ -2316,7 +2334,7 @@
         <v>1.0380000000000001E-3</v>
       </c>
       <c r="J43" s="11">
-        <f>1/I43</f>
+        <f t="shared" si="0"/>
         <v>963.39113680154139</v>
       </c>
       <c r="K43" s="8">
@@ -2326,7 +2344,7 @@
       <c r="M43" s="6"/>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="9"/>
       <c r="C44" s="10" t="s">
@@ -2351,7 +2369,7 @@
         <v>1.075E-3</v>
       </c>
       <c r="J44" s="11">
-        <f>1/I44</f>
+        <f t="shared" si="0"/>
         <v>930.23255813953483</v>
       </c>
       <c r="K44" s="8">
@@ -2361,7 +2379,7 @@
       <c r="M44" s="6"/>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="9"/>
       <c r="C45" s="10" t="s">
@@ -2386,7 +2404,7 @@
         <v>1.1050000000000001E-3</v>
       </c>
       <c r="J45" s="11">
-        <f>1/I45</f>
+        <f t="shared" ref="J45:J76" si="1">1/I45</f>
         <v>904.97737556561083</v>
       </c>
       <c r="K45" s="8">
@@ -2396,7 +2414,7 @@
       <c r="M45" s="6"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="9"/>
       <c r="C46" s="10" t="s">
@@ -2421,7 +2439,7 @@
         <v>1.073E-3</v>
       </c>
       <c r="J46" s="11">
-        <f>1/I46</f>
+        <f t="shared" si="1"/>
         <v>931.96644920782853</v>
       </c>
       <c r="K46" s="8">
@@ -2431,7 +2449,7 @@
       <c r="M46" s="6"/>
       <c r="N46" s="2"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="9"/>
       <c r="C47" s="10" t="s">
@@ -2456,7 +2474,7 @@
         <v>1.0640000000000001E-3</v>
       </c>
       <c r="J47" s="11">
-        <f>1/I47</f>
+        <f t="shared" si="1"/>
         <v>939.84962406015029</v>
       </c>
       <c r="K47" s="8">
@@ -2466,7 +2484,7 @@
       <c r="M47" s="6"/>
       <c r="N47" s="2"/>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="9"/>
       <c r="C48" s="10" t="s">
@@ -2491,7 +2509,7 @@
         <v>1.0809999999999999E-3</v>
       </c>
       <c r="J48" s="11">
-        <f>1/I48</f>
+        <f t="shared" si="1"/>
         <v>925.06938020351538</v>
       </c>
       <c r="K48" s="8">
@@ -2501,7 +2519,7 @@
       <c r="M48" s="6"/>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="9"/>
       <c r="C49" s="10" t="s">
@@ -2526,7 +2544,7 @@
         <v>9.7400000000000004E-3</v>
       </c>
       <c r="J49" s="11">
-        <f>1/I49</f>
+        <f t="shared" si="1"/>
         <v>102.6694045174538</v>
       </c>
       <c r="K49" s="8">
@@ -2536,7 +2554,7 @@
       <c r="M49" s="6"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="9"/>
       <c r="C50" s="10" t="s">
@@ -2561,7 +2579,7 @@
         <v>1.009E-2</v>
       </c>
       <c r="J50" s="11">
-        <f>1/I50</f>
+        <f t="shared" si="1"/>
         <v>99.108027750247771</v>
       </c>
       <c r="K50" s="8">
@@ -2571,7 +2589,7 @@
       <c r="M50" s="6"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="9"/>
       <c r="C51" s="10" t="s">
@@ -2596,7 +2614,7 @@
         <v>1.0149999999999999E-2</v>
       </c>
       <c r="J51" s="7">
-        <f>1/I51</f>
+        <f t="shared" si="1"/>
         <v>98.52216748768474</v>
       </c>
       <c r="K51" s="8">
@@ -2606,7 +2624,7 @@
       <c r="M51" s="6"/>
       <c r="N51" s="2"/>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="9"/>
       <c r="C52" s="10" t="s">
@@ -2631,7 +2649,7 @@
         <v>1.0659999999999999E-2</v>
       </c>
       <c r="J52" s="11">
-        <f>1/I52</f>
+        <f t="shared" si="1"/>
         <v>93.808630393996253</v>
       </c>
       <c r="K52" s="8">
@@ -2641,7 +2659,7 @@
       <c r="M52" s="6"/>
       <c r="N52" s="2"/>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="9"/>
       <c r="C53" s="10" t="s">
@@ -2666,7 +2684,7 @@
         <v>1.034E-2</v>
       </c>
       <c r="J53" s="11">
-        <f>1/I53</f>
+        <f t="shared" si="1"/>
         <v>96.71179883945841</v>
       </c>
       <c r="K53" s="8">
@@ -2676,7 +2694,7 @@
       <c r="M53" s="6"/>
       <c r="N53" s="2"/>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="9"/>
       <c r="C54" s="10" t="s">
@@ -2701,7 +2719,7 @@
         <v>1.0059999999999999E-2</v>
       </c>
       <c r="J54" s="13">
-        <f>1/I54</f>
+        <f t="shared" si="1"/>
         <v>99.40357852882704</v>
       </c>
       <c r="K54" s="8">
@@ -2711,7 +2729,7 @@
       <c r="M54" s="6"/>
       <c r="N54" s="2"/>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="9"/>
       <c r="C55" s="10" t="s">
@@ -2736,7 +2754,7 @@
         <v>1.0200000000000001E-2</v>
       </c>
       <c r="J55" s="11">
-        <f>1/I55</f>
+        <f t="shared" si="1"/>
         <v>98.039215686274503</v>
       </c>
       <c r="K55" s="8">
@@ -2746,7 +2764,7 @@
       <c r="M55" s="6"/>
       <c r="N55" s="2"/>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="9"/>
       <c r="C56" s="10" t="s">
@@ -2771,7 +2789,7 @@
         <v>9.9600000000000001E-3</v>
       </c>
       <c r="J56" s="11">
-        <f>1/I56</f>
+        <f t="shared" si="1"/>
         <v>100.40160642570281</v>
       </c>
       <c r="K56" s="8">
@@ -2781,7 +2799,7 @@
       <c r="M56" s="6"/>
       <c r="N56" s="2"/>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="9"/>
       <c r="C57" s="10" t="s">
@@ -2806,7 +2824,7 @@
         <v>1.0359999999999999E-2</v>
       </c>
       <c r="J57" s="11">
-        <f>1/I57</f>
+        <f t="shared" si="1"/>
         <v>96.525096525096529</v>
       </c>
       <c r="K57" s="8">
@@ -2816,7 +2834,7 @@
       <c r="M57" s="6"/>
       <c r="N57" s="2"/>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="9"/>
       <c r="C58" s="10" t="s">
@@ -2841,7 +2859,7 @@
         <v>9.8200000000000006E-3</v>
       </c>
       <c r="J58" s="11">
-        <f>1/I58</f>
+        <f t="shared" si="1"/>
         <v>101.83299389002036</v>
       </c>
       <c r="K58" s="8">
@@ -2851,7 +2869,7 @@
       <c r="M58" s="6"/>
       <c r="N58" s="2"/>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="9"/>
       <c r="C59" s="10" t="s">
@@ -2876,7 +2894,7 @@
         <v>1.0410000000000001E-2</v>
       </c>
       <c r="J59" s="11">
-        <f>1/I59</f>
+        <f t="shared" si="1"/>
         <v>96.061479346781937</v>
       </c>
       <c r="K59" s="8">
@@ -2886,7 +2904,7 @@
       <c r="M59" s="6"/>
       <c r="N59" s="2"/>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="9"/>
       <c r="C60" s="10" t="s">
@@ -2911,7 +2929,7 @@
         <v>9.9799999999999997E-4</v>
       </c>
       <c r="J60" s="11">
-        <f>1/I60</f>
+        <f t="shared" si="1"/>
         <v>1002.0040080160321</v>
       </c>
       <c r="K60" s="8">
@@ -2921,7 +2939,7 @@
       <c r="M60" s="6"/>
       <c r="N60" s="2"/>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="9"/>
       <c r="C61" s="10" t="s">
@@ -2946,7 +2964,7 @@
         <v>9.5699999999999995E-4</v>
       </c>
       <c r="J61" s="11">
-        <f>1/I61</f>
+        <f t="shared" si="1"/>
         <v>1044.9320794148382</v>
       </c>
       <c r="K61" s="8">
@@ -2956,7 +2974,7 @@
       <c r="M61" s="6"/>
       <c r="N61" s="2"/>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="9"/>
       <c r="C62" s="10" t="s">
@@ -2981,7 +2999,7 @@
         <v>1.0300000000000001E-3</v>
       </c>
       <c r="J62" s="11">
-        <f>1/I62</f>
+        <f t="shared" si="1"/>
         <v>970.87378640776694</v>
       </c>
       <c r="K62" s="8">
@@ -2991,7 +3009,7 @@
       <c r="M62" s="6"/>
       <c r="N62" s="2"/>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="9"/>
       <c r="C63" s="10" t="s">
@@ -3016,7 +3034,7 @@
         <v>9.8900000000000008E-4</v>
       </c>
       <c r="J63" s="11">
-        <f>1/I63</f>
+        <f t="shared" si="1"/>
         <v>1011.1223458038422</v>
       </c>
       <c r="K63" s="8">
@@ -3026,7 +3044,7 @@
       <c r="M63" s="6"/>
       <c r="N63" s="2"/>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="9"/>
       <c r="C64" s="10" t="s">
@@ -3051,7 +3069,7 @@
         <v>9.9299999999999996E-4</v>
       </c>
       <c r="J64" s="11">
-        <f>1/I64</f>
+        <f t="shared" si="1"/>
         <v>1007.0493454179256</v>
       </c>
       <c r="K64" s="8">
@@ -3061,7 +3079,7 @@
       <c r="M64" s="6"/>
       <c r="N64" s="2"/>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="9"/>
       <c r="C65" s="10" t="s">
@@ -3086,7 +3104,7 @@
         <v>1.016E-3</v>
       </c>
       <c r="J65" s="11">
-        <f>1/I65</f>
+        <f t="shared" si="1"/>
         <v>984.25196850393706</v>
       </c>
       <c r="K65" s="8">
@@ -3096,7 +3114,7 @@
       <c r="M65" s="6"/>
       <c r="N65" s="2"/>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="9"/>
       <c r="C66" s="10" t="s">
@@ -3121,7 +3139,7 @@
         <v>1.016E-3</v>
       </c>
       <c r="J66" s="11">
-        <f>1/I66</f>
+        <f t="shared" si="1"/>
         <v>984.25196850393706</v>
       </c>
       <c r="K66" s="8">
@@ -3131,7 +3149,7 @@
       <c r="M66" s="6"/>
       <c r="N66" s="2"/>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="9"/>
       <c r="C67" s="10" t="s">
@@ -3156,7 +3174,7 @@
         <v>1.0269999999999999E-3</v>
       </c>
       <c r="J67" s="11">
-        <f>1/I67</f>
+        <f t="shared" si="1"/>
         <v>973.70983446932826</v>
       </c>
       <c r="K67" s="8">
@@ -3166,7 +3184,7 @@
       <c r="M67" s="6"/>
       <c r="N67" s="2"/>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="9"/>
       <c r="C68" s="10" t="s">
@@ -3191,7 +3209,7 @@
         <v>1.011E-3</v>
       </c>
       <c r="J68" s="11">
-        <f>1/I68</f>
+        <f t="shared" si="1"/>
         <v>989.11968348170137</v>
       </c>
       <c r="K68" s="8">
@@ -3201,7 +3219,7 @@
       <c r="M68" s="6"/>
       <c r="N68" s="2"/>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="9"/>
       <c r="C69" s="10" t="s">
@@ -3226,7 +3244,7 @@
         <v>9.68E-4</v>
       </c>
       <c r="J69" s="11">
-        <f>1/I69</f>
+        <f t="shared" si="1"/>
         <v>1033.0578512396694</v>
       </c>
       <c r="K69" s="8">
@@ -3236,7 +3254,7 @@
       <c r="M69" s="6"/>
       <c r="N69" s="2"/>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="9"/>
       <c r="C70" s="10" t="s">
@@ -3261,7 +3279,7 @@
         <v>1.0549999999999999E-3</v>
       </c>
       <c r="J70" s="11">
-        <f>1/I70</f>
+        <f t="shared" si="1"/>
         <v>947.8672985781991</v>
       </c>
       <c r="K70" s="8">
@@ -3271,7 +3289,7 @@
       <c r="M70" s="6"/>
       <c r="N70" s="2"/>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="9"/>
       <c r="C71" s="10" t="s">
@@ -3296,7 +3314,7 @@
         <v>1.0399999999999999E-3</v>
       </c>
       <c r="J71" s="11">
-        <f>1/I71</f>
+        <f t="shared" si="1"/>
         <v>961.53846153846166</v>
       </c>
       <c r="K71" s="8">
@@ -3306,7 +3324,7 @@
       <c r="M71" s="6"/>
       <c r="N71" s="2"/>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="9"/>
       <c r="C72" s="10" t="s">
@@ -3331,7 +3349,7 @@
         <v>1.06E-3</v>
       </c>
       <c r="J72" s="11">
-        <f>1/I72</f>
+        <f t="shared" si="1"/>
         <v>943.39622641509436</v>
       </c>
       <c r="K72" s="8">
@@ -3341,7 +3359,7 @@
       <c r="M72" s="6"/>
       <c r="N72" s="2"/>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="9"/>
       <c r="C73" s="10" t="s">
@@ -3366,7 +3384,7 @@
         <v>1.024E-3</v>
       </c>
       <c r="J73" s="11">
-        <f>1/I73</f>
+        <f t="shared" si="1"/>
         <v>976.5625</v>
       </c>
       <c r="K73" s="8">
@@ -3376,7 +3394,7 @@
       <c r="M73" s="6"/>
       <c r="N73" s="2"/>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="9"/>
       <c r="C74" s="10" t="s">
@@ -3401,7 +3419,7 @@
         <v>1.0250000000000001E-3</v>
       </c>
       <c r="J74" s="11">
-        <f>1/I74</f>
+        <f t="shared" si="1"/>
         <v>975.60975609756088</v>
       </c>
       <c r="K74" s="8">
@@ -3411,7 +3429,7 @@
       <c r="M74" s="6"/>
       <c r="N74" s="2"/>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="9"/>
       <c r="C75" s="10" t="s">
@@ -3436,7 +3454,7 @@
         <v>9.3599999999999998E-4</v>
       </c>
       <c r="J75" s="11">
-        <f>1/I75</f>
+        <f t="shared" si="1"/>
         <v>1068.3760683760684</v>
       </c>
       <c r="K75" s="8">
@@ -3446,7 +3464,7 @@
       <c r="M75" s="6"/>
       <c r="N75" s="2"/>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="9"/>
       <c r="C76" s="10" t="s">
@@ -3471,7 +3489,7 @@
         <v>9.4899999999999997E-4</v>
       </c>
       <c r="J76" s="11">
-        <f>1/I76</f>
+        <f t="shared" si="1"/>
         <v>1053.7407797681772</v>
       </c>
       <c r="K76" s="8">
@@ -3481,7 +3499,7 @@
       <c r="M76" s="6"/>
       <c r="N76" s="2"/>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="9"/>
       <c r="C77" s="10" t="s">
@@ -3506,7 +3524,7 @@
         <v>9.4399999999999996E-4</v>
       </c>
       <c r="J77" s="11">
-        <f>1/I77</f>
+        <f t="shared" ref="J77:J92" si="2">1/I77</f>
         <v>1059.3220338983051</v>
       </c>
       <c r="K77" s="8">
@@ -3516,7 +3534,7 @@
       <c r="M77" s="6"/>
       <c r="N77" s="2"/>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="9"/>
       <c r="C78" s="10" t="s">
@@ -3541,7 +3559,7 @@
         <v>9.9599999999999992E-4</v>
       </c>
       <c r="J78" s="11">
-        <f>1/I78</f>
+        <f t="shared" si="2"/>
         <v>1004.0160642570282</v>
       </c>
       <c r="K78" s="8">
@@ -3551,7 +3569,7 @@
       <c r="M78" s="6"/>
       <c r="N78" s="2"/>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="9"/>
       <c r="C79" s="10" t="s">
@@ -3576,7 +3594,7 @@
         <v>1.0399999999999999E-3</v>
       </c>
       <c r="J79" s="11">
-        <f>1/I79</f>
+        <f t="shared" si="2"/>
         <v>961.53846153846166</v>
       </c>
       <c r="K79" s="8">
@@ -3586,7 +3604,7 @@
       <c r="M79" s="6"/>
       <c r="N79" s="2"/>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="9"/>
       <c r="C80" s="10" t="s">
@@ -3611,7 +3629,7 @@
         <v>9.5799999999999998E-4</v>
       </c>
       <c r="J80" s="11">
-        <f>1/I80</f>
+        <f t="shared" si="2"/>
         <v>1043.8413361169103</v>
       </c>
       <c r="K80" s="8">
@@ -3621,7 +3639,7 @@
       <c r="M80" s="6"/>
       <c r="N80" s="2"/>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="9"/>
       <c r="C81" s="10" t="s">
@@ -3646,7 +3664,7 @@
         <v>9.2900000000000003E-4</v>
       </c>
       <c r="J81" s="11">
-        <f>1/I81</f>
+        <f t="shared" si="2"/>
         <v>1076.4262648008612</v>
       </c>
       <c r="K81" s="8">
@@ -3656,7 +3674,7 @@
       <c r="M81" s="6"/>
       <c r="N81" s="2"/>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="9"/>
       <c r="C82" s="10" t="s">
@@ -3681,7 +3699,7 @@
         <v>9.5799999999999998E-4</v>
       </c>
       <c r="J82" s="11">
-        <f>1/I82</f>
+        <f t="shared" si="2"/>
         <v>1043.8413361169103</v>
       </c>
       <c r="K82" s="8">
@@ -3691,7 +3709,7 @@
       <c r="M82" s="6"/>
       <c r="N82" s="2"/>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="9"/>
       <c r="C83" s="10" t="s">
@@ -3716,7 +3734,7 @@
         <v>9.9700000000000006E-4</v>
       </c>
       <c r="J83" s="11">
-        <f>1/I83</f>
+        <f t="shared" si="2"/>
         <v>1003.0090270812436</v>
       </c>
       <c r="K83" s="8">
@@ -3726,7 +3744,7 @@
       <c r="M83" s="6"/>
       <c r="N83" s="2"/>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="9"/>
       <c r="C84" s="10" t="s">
@@ -3751,7 +3769,7 @@
         <v>9.8799999999999995E-4</v>
       </c>
       <c r="J84" s="11">
-        <f>1/I84</f>
+        <f t="shared" si="2"/>
         <v>1012.1457489878543</v>
       </c>
       <c r="K84" s="8">
@@ -3761,7 +3779,7 @@
       <c r="M84" s="6"/>
       <c r="N84" s="2"/>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="9"/>
       <c r="C85" s="10" t="s">
@@ -3786,7 +3804,7 @@
         <v>9.4399999999999996E-4</v>
       </c>
       <c r="J85" s="11">
-        <f>1/I85</f>
+        <f t="shared" si="2"/>
         <v>1059.3220338983051</v>
       </c>
       <c r="K85" s="8">
@@ -3796,7 +3814,7 @@
       <c r="M85" s="6"/>
       <c r="N85" s="2"/>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="9"/>
       <c r="C86" s="10" t="s">
@@ -3821,7 +3839,7 @@
         <v>1.008E-3</v>
       </c>
       <c r="J86" s="11">
-        <f>1/I86</f>
+        <f t="shared" si="2"/>
         <v>992.06349206349205</v>
       </c>
       <c r="K86" s="8">
@@ -3831,7 +3849,7 @@
       <c r="M86" s="6"/>
       <c r="N86" s="2"/>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="9"/>
       <c r="C87" s="10" t="s">
@@ -3856,7 +3874,7 @@
         <v>1.0449999999999999E-3</v>
       </c>
       <c r="J87" s="11">
-        <f>1/I87</f>
+        <f t="shared" si="2"/>
         <v>956.93779904306223</v>
       </c>
       <c r="K87" s="8">
@@ -3866,7 +3884,7 @@
       <c r="M87" s="6"/>
       <c r="N87" s="2"/>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="9"/>
       <c r="C88" s="10" t="s">
@@ -3891,7 +3909,7 @@
         <v>9.9200000000000004E-4</v>
       </c>
       <c r="J88" s="11">
-        <f>1/I88</f>
+        <f t="shared" si="2"/>
         <v>1008.0645161290322</v>
       </c>
       <c r="K88" s="8">
@@ -3901,7 +3919,7 @@
       <c r="M88" s="6"/>
       <c r="N88" s="2"/>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="9"/>
       <c r="C89" s="10" t="s">
@@ -3926,7 +3944,7 @@
         <v>9.8900000000000008E-4</v>
       </c>
       <c r="J89" s="31">
-        <f>1/I89</f>
+        <f t="shared" si="2"/>
         <v>1011.1223458038422</v>
       </c>
       <c r="K89" s="32">
@@ -3936,154 +3954,188 @@
       <c r="M89" s="6"/>
       <c r="N89" s="2"/>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="9"/>
-      <c r="C90" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D90" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E90" s="15">
-        <v>9999999</v>
-      </c>
-      <c r="F90" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="G90" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H90" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="I90" s="28">
-        <v>1</v>
-      </c>
-      <c r="J90" s="28">
-        <f>1/I90</f>
-        <v>1</v>
-      </c>
-      <c r="K90" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="L90" s="16"/>
+      <c r="C90" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E90" s="30">
+        <v>217463</v>
+      </c>
+      <c r="F90" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G90" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H90" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="I90" s="31">
+        <v>1.0120000000000001E-2</v>
+      </c>
+      <c r="J90" s="31">
+        <f t="shared" si="2"/>
+        <v>98.814229249011859</v>
+      </c>
+      <c r="K90" s="32">
+        <v>42738</v>
+      </c>
+      <c r="L90" s="12"/>
       <c r="M90" s="6"/>
       <c r="N90" s="2"/>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
-      <c r="B91" s="17"/>
-      <c r="C91" s="18"/>
-      <c r="D91" s="18"/>
-      <c r="E91" s="18"/>
-      <c r="F91" s="18"/>
-      <c r="G91" s="18"/>
-      <c r="H91" s="18"/>
-      <c r="I91" s="19"/>
-      <c r="J91" s="19"/>
-      <c r="K91" s="18"/>
-      <c r="L91" s="18"/>
-      <c r="M91" s="20"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E91" s="30">
+        <v>217649</v>
+      </c>
+      <c r="F91" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G91" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H91" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="I91" s="31">
+        <v>1.0070000000000001E-2</v>
+      </c>
+      <c r="J91" s="31">
+        <f t="shared" si="2"/>
+        <v>99.304865938430979</v>
+      </c>
+      <c r="K91" s="32">
+        <v>42741</v>
+      </c>
+      <c r="L91" s="12"/>
+      <c r="M91" s="6"/>
       <c r="N91" s="2"/>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
-      <c r="F92" s="2"/>
-      <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
-      <c r="I92" s="3"/>
-      <c r="J92" s="3"/>
-      <c r="K92" s="2"/>
-      <c r="L92" s="2"/>
-      <c r="M92" s="2"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E92" s="15">
+        <v>9999999</v>
+      </c>
+      <c r="F92" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G92" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H92" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="I92" s="28">
+        <v>1</v>
+      </c>
+      <c r="J92" s="28">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K92" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="L92" s="16"/>
+      <c r="M92" s="6"/>
       <c r="N92" s="2"/>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="3"/>
-      <c r="J93" s="3"/>
-      <c r="K93" s="2"/>
-      <c r="L93" s="2"/>
-      <c r="M93" s="2"/>
+      <c r="B93" s="17"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="18"/>
+      <c r="G93" s="18"/>
+      <c r="H93" s="18"/>
+      <c r="I93" s="19"/>
+      <c r="J93" s="19"/>
+      <c r="K93" s="18"/>
+      <c r="L93" s="18"/>
+      <c r="M93" s="20"/>
       <c r="N93" s="2"/>
     </row>
-    <row r="94" spans="1:14">
-      <c r="A94" s="21"/>
-      <c r="B94" s="22" t="s">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="2"/>
+      <c r="L94" s="2"/>
+      <c r="M94" s="2"/>
+      <c r="N94" s="2"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="2"/>
+      <c r="L95" s="2"/>
+      <c r="M95" s="2"/>
+      <c r="N95" s="2"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A96" s="21"/>
+      <c r="B96" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C94" s="22"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="22"/>
-      <c r="F94" s="22"/>
-      <c r="G94" s="22"/>
-      <c r="H94" s="22"/>
-      <c r="I94" s="23"/>
-      <c r="J94" s="23"/>
-      <c r="K94" s="22"/>
-      <c r="L94" s="22"/>
-      <c r="M94" s="22"/>
-      <c r="N94" s="22"/>
-    </row>
-    <row r="95" spans="1:14">
-      <c r="A95" s="4"/>
-      <c r="B95" s="24" t="s">
+      <c r="C96" s="22"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="22"/>
+      <c r="F96" s="22"/>
+      <c r="G96" s="22"/>
+      <c r="H96" s="22"/>
+      <c r="I96" s="23"/>
+      <c r="J96" s="23"/>
+      <c r="K96" s="22"/>
+      <c r="L96" s="22"/>
+      <c r="M96" s="22"/>
+      <c r="N96" s="22"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A97" s="4"/>
+      <c r="B97" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C95" s="24"/>
-      <c r="D95" s="24"/>
-      <c r="E95" s="24"/>
-      <c r="F95" s="24"/>
-      <c r="G95" s="24"/>
-      <c r="H95" s="24"/>
-      <c r="I95" s="25"/>
-      <c r="J95" s="25"/>
-      <c r="K95" s="24"/>
-      <c r="L95" s="24"/>
-      <c r="M95" s="24"/>
-      <c r="N95" s="24"/>
-    </row>
-    <row r="96" spans="1:14">
-      <c r="A96" s="4"/>
-      <c r="B96" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C96" s="24"/>
-      <c r="D96" s="24"/>
-      <c r="E96" s="24"/>
-      <c r="F96" s="24"/>
-      <c r="G96" s="24"/>
-      <c r="H96" s="24"/>
-      <c r="I96" s="25"/>
-      <c r="J96" s="25"/>
-      <c r="K96" s="24"/>
-      <c r="L96" s="24"/>
-      <c r="M96" s="24"/>
-      <c r="N96" s="24"/>
-    </row>
-    <row r="97" spans="1:14">
-      <c r="A97" s="4"/>
-      <c r="B97" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C97" s="26"/>
-      <c r="D97" s="26"/>
-      <c r="E97" s="26"/>
-      <c r="F97" s="26"/>
-      <c r="G97" s="26"/>
-      <c r="H97" s="26"/>
+      <c r="C97" s="24"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="24"/>
+      <c r="H97" s="24"/>
       <c r="I97" s="25"/>
       <c r="J97" s="25"/>
       <c r="K97" s="24"/>
@@ -4091,17 +4143,17 @@
       <c r="M97" s="24"/>
       <c r="N97" s="24"/>
     </row>
-    <row r="98" spans="1:14">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
-      <c r="B98" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C98" s="26"/>
-      <c r="D98" s="26"/>
-      <c r="E98" s="26"/>
-      <c r="F98" s="26"/>
-      <c r="G98" s="26"/>
-      <c r="H98" s="26"/>
+      <c r="B98" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C98" s="24"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="24"/>
+      <c r="H98" s="24"/>
       <c r="I98" s="25"/>
       <c r="J98" s="25"/>
       <c r="K98" s="24"/>
@@ -4109,10 +4161,10 @@
       <c r="M98" s="24"/>
       <c r="N98" s="24"/>
     </row>
-    <row r="99" spans="1:14">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C99" s="26"/>
       <c r="D99" s="26"/>
@@ -4127,51 +4179,88 @@
       <c r="M99" s="24"/>
       <c r="N99" s="24"/>
     </row>
-    <row r="100" spans="1:14">
-      <c r="A100" s="17"/>
-      <c r="B100" s="18" t="s">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
+      <c r="B100" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C100" s="26"/>
+      <c r="D100" s="26"/>
+      <c r="E100" s="26"/>
+      <c r="F100" s="26"/>
+      <c r="G100" s="26"/>
+      <c r="H100" s="26"/>
+      <c r="I100" s="25"/>
+      <c r="J100" s="25"/>
+      <c r="K100" s="24"/>
+      <c r="L100" s="24"/>
+      <c r="M100" s="24"/>
+      <c r="N100" s="24"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A101" s="4"/>
+      <c r="B101" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C101" s="26"/>
+      <c r="D101" s="26"/>
+      <c r="E101" s="26"/>
+      <c r="F101" s="26"/>
+      <c r="G101" s="26"/>
+      <c r="H101" s="26"/>
+      <c r="I101" s="25"/>
+      <c r="J101" s="25"/>
+      <c r="K101" s="24"/>
+      <c r="L101" s="24"/>
+      <c r="M101" s="24"/>
+      <c r="N101" s="24"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A102" s="17"/>
+      <c r="B102" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C100" s="18"/>
-      <c r="D100" s="18"/>
-      <c r="E100" s="18"/>
-      <c r="F100" s="18"/>
-      <c r="G100" s="18"/>
-      <c r="H100" s="18"/>
-      <c r="I100" s="19"/>
-      <c r="J100" s="19"/>
-      <c r="K100" s="18"/>
-      <c r="L100" s="18"/>
-      <c r="M100" s="18"/>
-      <c r="N100" s="18"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="18"/>
+      <c r="G102" s="18"/>
+      <c r="H102" s="18"/>
+      <c r="I102" s="19"/>
+      <c r="J102" s="19"/>
+      <c r="K102" s="18"/>
+      <c r="L102" s="18"/>
+      <c r="M102" s="18"/>
+      <c r="N102" s="18"/>
     </row>
   </sheetData>
   <sortState ref="C4:L90">
     <sortCondition ref="E4:E90"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>